<commit_message>
coloquei mais dados na planiha
</commit_message>
<xml_diff>
--- a/trabalho_peso3.xlsx
+++ b/trabalho_peso3.xlsx
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +403,7 @@
         <v>0.02</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B20" si="0">SIN(A3)</f>
+        <f t="shared" ref="B3:B66" si="0">SIN(A3)</f>
         <v>1.999866669333308E-2</v>
       </c>
     </row>
@@ -558,6 +558,726 @@
       <c r="B20">
         <f t="shared" si="0"/>
         <v>0.18885889497650057</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.2</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.19866933079506122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.20845989984609956</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.21822962308086932</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.22797752353518841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.23770262642713458</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.24740395925452294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0.25708055189215512</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0.26673143668883115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0.27635564856411376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.28595222510483553</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.3</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.29552020666133955</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0.3050586364434435</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0.31456656061611776</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0.32404302839486837</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0.3334870921408144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0.34289780745545134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>0.35227423327508994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>0.36161543196496199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>0.37092046941298268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>0.38018841512316143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.4</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>0.38941834230865052</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>0.39860932798442289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>0.40776045305957015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>0.41687080242921076</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>0.42593946506599961</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>0.43496553411123023</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>0.44394810696551978</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>0.45288628537906828</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>0.4617791755414829</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>0.47062588817115802</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0.5</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>0.47942553860420301</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0.51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>0.48817724688290748</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>0.49688013784373675</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>0.50553334120484694</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0.54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>0.51413599165311319</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>0.52268722893065922</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>0.5311861979208834</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>0.53963204873396919</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>0.54802393679187356</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0.59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>0.55636102291278378</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0.6</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>0.56464247339503537</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>0.57286746010048128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.62</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>0.58103516053730508</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0.63</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>0.5891447579422695</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.64</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>0.59719544136239211</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.65</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>0.60518640573603955</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.66</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B100" si="1">SIN(A67)</f>
+        <v>0.6131168519734338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.67</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>0.62098598703655972</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.68</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>0.62879302401846859</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.69</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>0.63653718222196787</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0.7</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>0.64421768723769102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0.71</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>0.65183377102153661</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0.72</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>0.6593846719714731</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0.73</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>0.66686963500369789</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.74</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>0.67428791162814505</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0.750000000000001</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>0.6816387600233349</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0.76000000000000101</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>0.68892144511055209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0.77000000000000102</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>0.69613523862735749</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0.78000000000000103</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>0.70327941920041093</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0.79000000000000103</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>0.71035327241760848</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0.80000000000000104</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>0.71735609089952346</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0.81000000000000105</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="1"/>
+        <v>0.72428717437014323</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0.82000000000000095</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>0.73114582972689657</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0.83000000000000096</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>0.73793137110996332</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0.84000000000000097</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>0.74464311997085997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0.85000000000000098</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>0.75128040514029337</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0.86000000000000099</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>0.75784256289527763</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.87000000000000099</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>0.76432893702550575</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0.880000000000001</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>0.77073887889896997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0.89000000000000101</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>0.77707174752682451</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0.90000000000000102</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>0.78332690962748397</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0.91000000000000103</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>0.78950373968995102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0.92000000000000104</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="1"/>
+        <v>0.7956016200363667</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0.93000000000000105</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="1"/>
+        <v>0.80161994088377775</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0.94000000000000095</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="1"/>
+        <v>0.80755810040511489</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>0.95000000000000095</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="1"/>
+        <v>0.8134155047893743</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0.96000000000000096</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="1"/>
+        <v>0.81919156830099882</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0.97000000000000097</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="1"/>
+        <v>0.82488571333845062</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0.98000000000000098</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="1"/>
+        <v>0.83049737049197103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0.99000000000000099</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="1"/>
+        <v>0.83602597860052108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>